<commit_message>
fix bug import, tambah kolom type di import germination
</commit_message>
<xml_diff>
--- a/storage/app/public/form_import/form_import_germin.xlsx
+++ b/storage/app/public/form_import/form_import_germin.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aldhi/Documents/Storage/Dev/laravel/08-socfin-sawit/storage/app/public/form_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A703F548-4BB1-6F4A-BF60-E23279F9B5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8BC088-1029-1742-B058-3C5CDB4CB11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14380" yWindow="31260" windowWidth="25700" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>ID Initiation</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Jlh Botol Germin</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>Germination</t>
   </si>
 </sst>
 </file>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E47813-669A-4B4E-A009-96C1097A77F5}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -462,11 +474,11 @@
     <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="8" max="9" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -491,8 +503,11 @@
       <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -517,8 +532,11 @@
       <c r="H2" s="2">
         <v>2</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -543,9 +561,41 @@
       <c r="H3" s="2">
         <v>1</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>400</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>